<commit_message>
added my WIP answers and updated over/under living stark children in answer key
</commit_message>
<xml_diff>
--- a/data-raw/answer-key.xlsx
+++ b/data-raw/answer-key.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5778308-F8A6-4316-97EE-37B70660FE21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA06F19-A78F-4882-90DD-D73FAB2D3E34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,23 +735,23 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1930,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:IT43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
@@ -1943,13 +1943,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1">
       <c r="A2" s="4"/>
@@ -2391,11 +2391,11 @@
     </row>
     <row r="26" spans="1:8" ht="20.85" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="19"/>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -2403,11 +2403,11 @@
     </row>
     <row r="27" spans="1:8" ht="20.85" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="19"/>
       <c r="H27" s="3" t="s">
         <v>11</v>
@@ -2415,11 +2415,11 @@
     </row>
     <row r="28" spans="1:8" ht="20.85" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="15"/>
       <c r="H28" s="3" t="s">
         <v>13</v>
@@ -2427,11 +2427,11 @@
     </row>
     <row r="29" spans="1:8" ht="32.1" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="19"/>
       <c r="H29" s="3" t="s">
         <v>15</v>
@@ -2439,11 +2439,11 @@
     </row>
     <row r="30" spans="1:8" ht="30.95" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="19"/>
       <c r="H30" s="3" t="s">
         <v>17</v>
@@ -2451,11 +2451,11 @@
     </row>
     <row r="31" spans="1:8" ht="23.1" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="15"/>
       <c r="H31" s="3" t="s">
         <v>19</v>
@@ -2463,13 +2463,13 @@
     </row>
     <row r="32" spans="1:8" ht="23.1" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>21</v>
@@ -2477,11 +2477,11 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -2491,11 +2491,11 @@
     </row>
     <row r="34" spans="1:8" ht="32.85" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="19"/>
       <c r="H34" s="3" t="s">
         <v>27</v>
@@ -2548,6 +2548,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -2555,11 +2560,6 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">

</xml_diff>

<commit_message>
updated answer key because ghost is alive
</commit_message>
<xml_diff>
--- a/data-raw/answer-key.xlsx
+++ b/data-raw/answer-key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7AAE83-2786-4A52-9043-53445F8FF331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1805E1-3EF7-4CD8-9DC3-068B9983CF3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,23 +735,23 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1931,7 +1931,7 @@
   <dimension ref="A1:IT43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
@@ -1943,13 +1943,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1">
       <c r="A2" s="4"/>
@@ -2253,7 +2253,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>33</v>
@@ -2391,13 +2391,13 @@
     </row>
     <row r="26" spans="1:8" ht="20.85" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="19" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -2405,11 +2405,11 @@
     </row>
     <row r="27" spans="1:8" ht="20.85" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="19"/>
       <c r="H27" s="3" t="s">
         <v>11</v>
@@ -2417,11 +2417,11 @@
     </row>
     <row r="28" spans="1:8" ht="20.85" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="15"/>
       <c r="H28" s="3" t="s">
         <v>13</v>
@@ -2429,11 +2429,11 @@
     </row>
     <row r="29" spans="1:8" ht="32.1" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="19" t="s">
         <v>8</v>
       </c>
@@ -2443,11 +2443,11 @@
     </row>
     <row r="30" spans="1:8" ht="30.95" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="19"/>
       <c r="H30" s="3" t="s">
         <v>17</v>
@@ -2455,11 +2455,11 @@
     </row>
     <row r="31" spans="1:8" ht="23.1" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="15" t="s">
         <v>51</v>
       </c>
@@ -2469,11 +2469,11 @@
     </row>
     <row r="32" spans="1:8" ht="23.1" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="16" t="s">
         <v>53</v>
       </c>
@@ -2483,11 +2483,11 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -2497,11 +2497,11 @@
     </row>
     <row r="34" spans="1:8" ht="32.85" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="19"/>
       <c r="H34" s="3" t="s">
         <v>27</v>
@@ -2554,6 +2554,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -2561,11 +2566,6 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">

</xml_diff>

<commit_message>
updated answer key for ep 5
</commit_message>
<xml_diff>
--- a/data-raw/answer-key.xlsx
+++ b/data-raw/answer-key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E677B96-4212-4221-A730-35E460138785}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD51ED8-CB7D-42FD-8702-08C1309C2AAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="63">
   <si>
     <t>Table 1</t>
   </si>
@@ -735,23 +735,23 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1930,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:IT43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
@@ -1943,13 +1943,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1">
       <c r="A2" s="4"/>
@@ -2001,7 +2001,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>4</v>
@@ -2043,7 +2043,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>11</v>
@@ -2109,7 +2109,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>23</v>
@@ -2169,7 +2169,7 @@
         <v>23</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
@@ -2259,7 +2259,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>34</v>
@@ -2331,7 +2331,7 @@
         <v>41</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>42</v>
@@ -2349,7 +2349,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>44</v>
@@ -2391,11 +2391,11 @@
     </row>
     <row r="26" spans="1:8" ht="20.85" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="19" t="s">
         <v>13</v>
       </c>
@@ -2405,11 +2405,11 @@
     </row>
     <row r="27" spans="1:8" ht="20.85" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="19"/>
       <c r="H27" s="3" t="s">
         <v>11</v>
@@ -2417,23 +2417,25 @@
     </row>
     <row r="28" spans="1:8" ht="20.85" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="15"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="H28" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="32.1" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="19" t="s">
         <v>8</v>
       </c>
@@ -2443,23 +2445,25 @@
     </row>
     <row r="30" spans="1:8" ht="30.95" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="H30" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="23.1" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="15" t="s">
         <v>51</v>
       </c>
@@ -2469,11 +2473,11 @@
     </row>
     <row r="32" spans="1:8" ht="23.1" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="16" t="s">
         <v>53</v>
       </c>
@@ -2483,11 +2487,11 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -2497,11 +2501,11 @@
     </row>
     <row r="34" spans="1:8" ht="32.85" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="19"/>
       <c r="H34" s="3" t="s">
         <v>27</v>
@@ -2554,6 +2558,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -2561,11 +2570,6 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">

</xml_diff>

<commit_message>
updated for the worst episode ever
</commit_message>
<xml_diff>
--- a/data-raw/answer-key.xlsx
+++ b/data-raw/answer-key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD51ED8-CB7D-42FD-8702-08C1309C2AAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8782DA95-3241-4096-930E-6A43E2B8235E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
   <si>
     <t>Table 1</t>
   </si>
@@ -735,23 +735,23 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1930,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:IT43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
@@ -1943,13 +1943,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.6" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1">
       <c r="A2" s="4"/>
@@ -2163,7 +2163,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>23</v>
@@ -2391,11 +2391,11 @@
     </row>
     <row r="26" spans="1:8" ht="20.85" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="19" t="s">
         <v>13</v>
       </c>
@@ -2405,23 +2405,25 @@
     </row>
     <row r="27" spans="1:8" ht="20.85" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="19"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.85" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="15" t="s">
         <v>7</v>
       </c>
@@ -2431,11 +2433,11 @@
     </row>
     <row r="29" spans="1:8" ht="32.1" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="19" t="s">
         <v>8</v>
       </c>
@@ -2445,11 +2447,11 @@
     </row>
     <row r="30" spans="1:8" ht="30.95" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="19" t="s">
         <v>22</v>
       </c>
@@ -2459,11 +2461,11 @@
     </row>
     <row r="31" spans="1:8" ht="23.1" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="15" t="s">
         <v>51</v>
       </c>
@@ -2473,11 +2475,11 @@
     </row>
     <row r="32" spans="1:8" ht="23.1" customHeight="1">
       <c r="A32" s="8"/>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="16" t="s">
         <v>53</v>
       </c>
@@ -2487,11 +2489,11 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1">
       <c r="A33" s="8"/>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="16" t="s">
         <v>52</v>
       </c>
@@ -2501,12 +2503,14 @@
     </row>
     <row r="34" spans="1:8" ht="32.85" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="19"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="H34" s="3" t="s">
         <v>27</v>
       </c>
@@ -2558,11 +2562,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
@@ -2570,6 +2569,11 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">

</xml_diff>